<commit_message>
ignoring rider folder, added for illustration purposes
</commit_message>
<xml_diff>
--- a/Assets/Cards.xlsx
+++ b/Assets/Cards.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity Projects\Virtual Deck\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity Projects\VirtualDeck\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E6A68A-94BD-45E8-98E7-55D294C84326}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF769A9-0912-4CAC-94F3-E61975B1A87E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1950" windowWidth="21585" windowHeight="11385" activeTab="1" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
+    <workbookView xWindow="4620" yWindow="915" windowWidth="21585" windowHeight="11385" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
   </bookViews>
   <sheets>
     <sheet name="Card Library" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>Spider man is going around killing people a lot!</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>yummmmmy</t>
   </si>
 </sst>
 </file>
@@ -437,16 +443,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374E0025-F2D2-430F-ABA1-AEDCA1230C58}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="95.140625" customWidth="1"/>
+    <col min="2" max="2" width="47.140625" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
   </cols>
@@ -539,6 +545,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -546,10 +563,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666581B7-BE17-437B-B40C-D534B472B9DC}">
-  <dimension ref="A2:C7"/>
+  <dimension ref="A2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,6 +640,28 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added functionality for loading art assets from Addressables
</commit_message>
<xml_diff>
--- a/Assets/Cards.xlsx
+++ b/Assets/Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity Projects\VirtualDeck\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF769A9-0912-4CAC-94F3-E61975B1A87E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B1113A-21F4-4B98-97CE-F98E552DF861}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="915" windowWidth="21585" windowHeight="11385" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
   </bookViews>
   <sheets>
     <sheet name="Card Library" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>Title</t>
   </si>
@@ -92,6 +92,84 @@
   </si>
   <si>
     <t>yummmmmy</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>fire-breath</t>
+  </si>
+  <si>
+    <t>ghost-ally</t>
+  </si>
+  <si>
+    <t>fire-dash</t>
+  </si>
+  <si>
+    <t>half-heart</t>
+  </si>
+  <si>
+    <t>stiletto</t>
+  </si>
+  <si>
+    <t>fire-silhouette</t>
+  </si>
+  <si>
+    <t>spider-mask</t>
+  </si>
+  <si>
+    <t>peach</t>
+  </si>
+  <si>
+    <t>skull-staff</t>
+  </si>
+  <si>
+    <t>Flame Bash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charge forwards in a ball of fire (Deal 10 dmg, Gain 5 Speed) </t>
+  </si>
+  <si>
+    <t>Dragon Breath</t>
+  </si>
+  <si>
+    <t>Unleash a breath of fire on a target dealing 12 dmg</t>
+  </si>
+  <si>
+    <t>Strawberry</t>
+  </si>
+  <si>
+    <t>Heals 10 hp (Consume)</t>
+  </si>
+  <si>
+    <t>Motion Sickness</t>
+  </si>
+  <si>
+    <t>Reduce target speed by 15</t>
+  </si>
+  <si>
+    <t>vomiting</t>
+  </si>
+  <si>
+    <t>Map it Out</t>
+  </si>
+  <si>
+    <t>Gain 7 speed</t>
+  </si>
+  <si>
+    <t>slalom</t>
+  </si>
+  <si>
+    <t>strawberry</t>
+  </si>
+  <si>
+    <t>Card Type</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Equipment</t>
   </si>
 </sst>
 </file>
@@ -443,21 +521,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374E0025-F2D2-430F-ABA1-AEDCA1230C58}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="47.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +547,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -478,8 +564,14 @@
       <c r="C2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -489,8 +581,14 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -500,8 +598,14 @@
       <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -511,8 +615,14 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -520,10 +630,16 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -533,8 +649,14 @@
       <c r="C7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -544,8 +666,14 @@
       <c r="C8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -555,18 +683,114 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E14" xr:uid="{3F624CD8-9735-48FD-AF23-C16505D64EC3}">
+      <formula1>"Skill, Equipment, Summon"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666581B7-BE17-437B-B40C-D534B472B9DC}">
-  <dimension ref="A2:C9"/>
+  <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +847,7 @@
         <v>12</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -656,10 +880,65 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug with excel sheet
</commit_message>
<xml_diff>
--- a/Assets/Cards.xlsx
+++ b/Assets/Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity Projects\VirtualDeck\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B1113A-21F4-4B98-97CE-F98E552DF861}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8941BA-072D-464E-BD4A-014A0889D991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
   </bookViews>
   <sheets>
     <sheet name="Card Library" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>Title</t>
   </si>
@@ -161,15 +161,6 @@
   </si>
   <si>
     <t>strawberry</t>
-  </si>
-  <si>
-    <t>Card Type</t>
-  </si>
-  <si>
-    <t>Skill</t>
-  </si>
-  <si>
-    <t>Equipment</t>
   </si>
 </sst>
 </file>
@@ -521,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374E0025-F2D2-430F-ABA1-AEDCA1230C58}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E1:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,7 +528,7 @@
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -550,11 +541,8 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -567,11 +555,8 @@
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -584,11 +569,8 @@
       <c r="D3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -601,11 +583,8 @@
       <c r="D4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -618,11 +597,8 @@
       <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -635,11 +611,8 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -652,11 +625,8 @@
       <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -669,11 +639,8 @@
       <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -686,11 +653,8 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -703,11 +667,8 @@
       <c r="D10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -720,11 +681,8 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -737,11 +695,8 @@
       <c r="D12" t="s">
         <v>41</v>
       </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -754,11 +709,8 @@
       <c r="D13" t="s">
         <v>37</v>
       </c>
-      <c r="E13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -770,9 +722,6 @@
       </c>
       <c r="D14" t="s">
         <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -789,7 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666581B7-BE17-437B-B40C-D534B472B9DC}">
   <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Setup basic  console UI and entity data
</commit_message>
<xml_diff>
--- a/Assets/Cards.xlsx
+++ b/Assets/Cards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity Projects\VirtualDeck\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8941BA-072D-464E-BD4A-014A0889D991}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CC7107-3D07-4580-91A9-E38377D4D60F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
   </bookViews>
   <sheets>
     <sheet name="Card Library" sheetId="1" r:id="rId1"/>
@@ -49,30 +49,15 @@
     <t>Ghost Clone</t>
   </si>
   <si>
-    <t>A staple weapon for the sneaky assassin</t>
-  </si>
-  <si>
     <t>Stiletto</t>
   </si>
   <si>
     <t>Staff of Death</t>
   </si>
   <si>
-    <t xml:space="preserve">Powerful.  Deadly. Terrifying. Only the truly desperate or greedy would dare wield this weapon. </t>
-  </si>
-  <si>
     <t>Piercing Stab</t>
   </si>
   <si>
-    <t>I'm feeling too lazy to try on this one</t>
-  </si>
-  <si>
-    <t>even after all their friends have been slain, the mage who knows ghost clone is never left standing alone</t>
-  </si>
-  <si>
-    <t>Oooo....Soothing... better than a day at the spa</t>
-  </si>
-  <si>
     <t>Heal</t>
   </si>
   <si>
@@ -82,18 +67,9 @@
     <t>SpiderMan slays</t>
   </si>
   <si>
-    <t>dance dance dance! I like to prance</t>
-  </si>
-  <si>
-    <t>Spider man is going around killing people a lot!</t>
-  </si>
-  <si>
     <t>Mango</t>
   </si>
   <si>
-    <t>yummmmmy</t>
-  </si>
-  <si>
     <t>Art</t>
   </si>
   <si>
@@ -161,6 +137,30 @@
   </si>
   <si>
     <t>strawberry</t>
+  </si>
+  <si>
+    <t>Spider man gives you 20 speed</t>
+  </si>
+  <si>
+    <t>Gain 20 hp (Consume)</t>
+  </si>
+  <si>
+    <t>dance dance dance! Ally gains 20 speed</t>
+  </si>
+  <si>
+    <t>Heal 5 for the next 3 turns</t>
+  </si>
+  <si>
+    <t>Powerful.  Deadly. Terrifying. If hp is less than 40 set hp to 0</t>
+  </si>
+  <si>
+    <t>summon a clone of yourself with 1 hp</t>
+  </si>
+  <si>
+    <t>Attack for 25 dmg</t>
+  </si>
+  <si>
+    <t>Attack for 14 dmg</t>
   </si>
 </sst>
 </file>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374E0025-F2D2-430F-ABA1-AEDCA1230C58}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E1:E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -547,181 +547,181 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666581B7-BE17-437B-B40C-D534B472B9DC}">
   <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +760,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -782,7 +782,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -793,10 +793,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -804,10 +804,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -815,7 +815,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -826,10 +826,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -837,7 +837,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -848,7 +848,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -881,7 +881,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <v>4</v>

</xml_diff>

<commit_message>
Refactoring based on recommendations from book clean code
-refactored console class
-refactoring game entities class

-sorry there is so much extra crap, I didn't commit for a while and this is the result
</commit_message>
<xml_diff>
--- a/Assets/Cards.xlsx
+++ b/Assets/Cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity Projects\VirtualDeck\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CC7107-3D07-4580-91A9-E38377D4D60F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB4DB55-609B-4075-9057-A652C171BB55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ED7B16DB-84E7-48C3-84C1-613E7AFBFD82}"/>
   </bookViews>
   <sheets>
     <sheet name="Card Library" sheetId="1" r:id="rId1"/>
@@ -514,15 +514,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{374E0025-F2D2-430F-ABA1-AEDCA1230C58}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{666581B7-BE17-437B-B40C-D534B472B9DC}">
   <dimension ref="A2:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>